<commit_message>
Add incomplete CSV version
</commit_message>
<xml_diff>
--- a/inc/flattened/createYaml/VTI.xlsx
+++ b/inc/flattened/createYaml/VTI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopherhammerly/giellalt/lang-ciw/inc/flattened/createYaml/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A49E82-2B25-534C-89F7-95579B511A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A89298-B5D7-594E-A44C-84BA47789016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1880" yWindow="3560" windowWidth="27320" windowHeight="14860" activeTab="1" xr2:uid="{B3487B63-25A5-BB42-95F2-8056A59367C3}"/>
+    <workbookView xWindow="1880" yWindow="3560" windowWidth="27320" windowHeight="14860" xr2:uid="{B3487B63-25A5-BB42-95F2-8056A59367C3}"/>
   </bookViews>
   <sheets>
     <sheet name="VTI_IND" sheetId="1" r:id="rId1"/>
@@ -2589,8 +2589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01A13B67-2206-C24E-B77C-511E4224659A}">
   <dimension ref="A1:L581"/>
   <sheetViews>
-    <sheetView topLeftCell="A430" zoomScale="109" workbookViewId="0">
-      <selection activeCell="D445" sqref="D445:D581"/>
+    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20987,8 +20987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C464A0D-9499-3742-9866-F8A002038C62}">
   <dimension ref="A1:L261"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A174" zoomScale="172" workbookViewId="0">
-      <selection activeCell="D183" sqref="D183:D261"/>
+    <sheetView zoomScale="172" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -29320,12 +29320,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -29494,15 +29491,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B87906FA-555E-44FE-8CE8-286F6253717E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2FEF8D93-91CB-4159-853C-C3180DA1A0F8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="b103a3be-6c61-44b0-93c5-2b779aa38a01"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="56612388-9f28-4625-93a0-6879c02082d6"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -29527,18 +29536,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2FEF8D93-91CB-4159-853C-C3180DA1A0F8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B87906FA-555E-44FE-8CE8-286F6253717E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="b103a3be-6c61-44b0-93c5-2b779aa38a01"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="56612388-9f28-4625-93a0-6879c02082d6"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>